<commit_message>
se terminaron las mediciones
</commit_message>
<xml_diff>
--- a/Ej1/Mediciones/ej1-ca-c1.xlsx
+++ b/Ej1/Mediciones/ej1-ca-c1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sony\Desktop\Ej1\Mediciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sony\Documents\GitHub\TC_TP2\Ej1\Mediciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="7">
   <si>
     <t>circuito 1  - caso 1 x10</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>circuito 1  - caso 1x1</t>
-  </si>
-  <si>
-    <t>400 (SON cuatrocientos)</t>
   </si>
 </sst>
 </file>
@@ -476,11 +473,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="316134064"/>
-        <c:axId val="316124816"/>
+        <c:axId val="-1778775184"/>
+        <c:axId val="-1778776816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="316134064"/>
+        <c:axId val="-1778775184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -523,7 +520,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316124816"/>
+        <c:crossAx val="-1778776816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -531,7 +528,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="316124816"/>
+        <c:axId val="-1778776816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -582,7 +579,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316134064"/>
+        <c:crossAx val="-1778775184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1487,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E46"/>
+    <sheetView tabSelected="1" topLeftCell="M6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC6" activeCellId="1" sqref="Y6:AA30 AC6:AC30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,21 +1718,9 @@
       <c r="T5">
         <v>60</v>
       </c>
-      <c r="Y5">
-        <v>1000</v>
-      </c>
-      <c r="Z5">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="AA5">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="AB5" s="2">
-        <f t="shared" ref="AB5:AB38" si="5">20*LOG10(AA5/Z5)</f>
-        <v>-19.157384135460852</v>
-      </c>
-      <c r="AC5">
-        <v>120</v>
+      <c r="AB5" s="2" t="e">
+        <f t="shared" ref="AB5:AB37" si="5">20*LOG10(AA5/Z5)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1775,20 +1760,20 @@
         <v>100</v>
       </c>
       <c r="Y6">
-        <v>1100</v>
+        <v>100</v>
       </c>
       <c r="Z6">
-        <v>0.48</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="AA6">
-        <v>5.1999999999999998E-2</v>
+        <v>0.02</v>
       </c>
       <c r="AB6" s="2">
         <f t="shared" si="5"/>
-        <v>-19.30475787481576</v>
+        <v>-19.95646161491451</v>
       </c>
       <c r="AC6">
-        <v>111</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
@@ -1840,20 +1825,20 @@
         <v>150</v>
       </c>
       <c r="Y7">
-        <v>1200</v>
+        <v>200</v>
       </c>
       <c r="Z7">
-        <v>0.48</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="AA7">
-        <v>0.05</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB7" s="2">
         <f t="shared" si="5"/>
-        <v>-19.64542466079137</v>
+        <v>-19.619535253731392</v>
       </c>
       <c r="AC7">
-        <v>102</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -1892,20 +1877,20 @@
         <v>200</v>
       </c>
       <c r="Y8">
-        <v>1300</v>
+        <v>300</v>
       </c>
       <c r="Z8">
-        <v>0.47899999999999998</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="AA8">
-        <v>4.8000000000000001E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB8" s="2">
         <f t="shared" si="5"/>
-        <v>-19.981885520779517</v>
+        <v>-19.619535253731392</v>
       </c>
       <c r="AC8">
-        <v>93</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -1944,20 +1929,20 @@
         <v>250</v>
       </c>
       <c r="Y9">
-        <v>1400</v>
+        <v>400</v>
       </c>
       <c r="Z9">
-        <v>0.47699999999999998</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="AA9">
-        <v>4.4999999999999998E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB9" s="2">
         <f t="shared" si="5"/>
-        <v>-20.506117305295405</v>
+        <v>-19.619535253731392</v>
       </c>
       <c r="AC9">
-        <v>85</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
@@ -2009,20 +1994,20 @@
         <v>300</v>
       </c>
       <c r="Y10">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="Z10">
-        <v>0.47699999999999998</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="AA10">
-        <v>4.2000000000000003E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB10" s="2">
         <f t="shared" si="5"/>
-        <v>-21.105381772844268</v>
+        <v>-19.619535253731392</v>
       </c>
       <c r="AC10">
-        <v>78</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
@@ -2074,20 +2059,20 @@
         <v>320</v>
       </c>
       <c r="Y11">
-        <v>1600</v>
+        <v>600</v>
       </c>
       <c r="Z11">
-        <v>0.47499999999999998</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="AA11">
-        <v>3.9E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB11" s="2">
         <f t="shared" si="5"/>
-        <v>-21.712580051967343</v>
+        <v>-19.619535253731392</v>
       </c>
       <c r="AC11">
-        <v>70</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
@@ -2139,20 +2124,20 @@
         <v>330</v>
       </c>
       <c r="Y12">
-        <v>1700</v>
+        <v>700</v>
       </c>
       <c r="Z12">
-        <v>0.47399999999999998</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="AA12">
-        <v>3.5999999999999997E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB12" s="2">
         <f t="shared" si="5"/>
-        <v>-22.389516818135956</v>
+        <v>-19.619535253731392</v>
       </c>
       <c r="AC12">
-        <v>65</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
@@ -2204,20 +2189,20 @@
         <v>340</v>
       </c>
       <c r="Y13">
-        <v>1750</v>
+        <v>800</v>
       </c>
       <c r="Z13">
-        <v>0.47299999999999998</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="AA13">
-        <v>3.5000000000000003E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB13" s="2">
-        <f t="shared" si="5"/>
-        <v>-22.615861927750718</v>
+        <f>20*LOG10(AA13/Z13)</f>
+        <v>-19.619535253731392</v>
       </c>
       <c r="AC13">
-        <v>62</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
@@ -2269,20 +2254,20 @@
         <v>350</v>
       </c>
       <c r="Y14">
-        <v>1780</v>
+        <v>900</v>
       </c>
       <c r="Z14">
-        <v>0.47299999999999998</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="AA14">
-        <v>3.4000000000000002E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB14" s="2">
         <f t="shared" si="5"/>
-        <v>-22.867644473911128</v>
+        <v>-19.662641494254089</v>
       </c>
       <c r="AC14">
-        <v>61</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
@@ -2334,20 +2319,20 @@
         <v>360</v>
       </c>
       <c r="Y15">
-        <v>1800</v>
+        <v>950</v>
       </c>
       <c r="Z15">
-        <v>0.47299999999999998</v>
+        <v>0.20200000000000001</v>
       </c>
       <c r="AA15">
-        <v>3.4000000000000002E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB15" s="2">
         <f t="shared" si="5"/>
-        <v>-22.867644473911128</v>
+        <v>-19.662641494254089</v>
       </c>
       <c r="AC15">
-        <v>59</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
@@ -2399,20 +2384,20 @@
         <v>370</v>
       </c>
       <c r="Y16">
-        <v>1900</v>
+        <v>1000</v>
       </c>
       <c r="Z16">
-        <v>0.47199999999999998</v>
+        <v>0.48099999999999998</v>
       </c>
       <c r="AA16">
-        <v>3.1E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="AB16" s="2">
         <f t="shared" si="5"/>
-        <v>-23.651606095996303</v>
+        <v>-19.157384135460852</v>
       </c>
       <c r="AC16">
-        <v>54</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
@@ -2464,20 +2449,20 @@
         <v>380</v>
       </c>
       <c r="Y17">
-        <v>2000</v>
+        <v>1100</v>
       </c>
       <c r="Z17">
-        <v>0.46899999999999997</v>
+        <v>0.48</v>
       </c>
       <c r="AA17">
-        <v>0.03</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="AB17" s="2">
         <f t="shared" si="5"/>
-        <v>-23.881031759908417</v>
+        <v>-19.30475787481576</v>
       </c>
       <c r="AC17">
-        <v>50</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
@@ -2529,20 +2514,20 @@
         <v>390</v>
       </c>
       <c r="Y18">
-        <v>2500</v>
+        <v>1200</v>
       </c>
       <c r="Z18">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="AA18">
-        <v>2.1000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AB18" s="2">
         <f t="shared" si="5"/>
-        <v>-26.810770738953096</v>
+        <v>-19.64542466079137</v>
       </c>
       <c r="AC18">
-        <v>34</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
@@ -2594,20 +2579,20 @@
         <v>400</v>
       </c>
       <c r="Y19">
-        <v>3000</v>
+        <v>1300</v>
       </c>
       <c r="Z19">
-        <v>0.45100000000000001</v>
+        <v>0.47899999999999998</v>
       </c>
       <c r="AA19">
-        <v>1.6E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="AB19" s="2">
         <f t="shared" si="5"/>
-        <v>-29.001131184440716</v>
+        <v>-19.981885520779517</v>
       </c>
       <c r="AC19">
-        <v>20</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
@@ -2658,21 +2643,21 @@
       <c r="T20">
         <v>410</v>
       </c>
-      <c r="Y20" t="s">
-        <v>7</v>
+      <c r="Y20">
+        <v>1400</v>
       </c>
       <c r="Z20">
-        <v>0.96699999999999997</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="AA20">
-        <v>0.1</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AB20" s="2">
         <f t="shared" si="5"/>
-        <v>-19.708529481660033</v>
+        <v>-20.506117305295405</v>
       </c>
       <c r="AC20">
-        <v>160</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
@@ -2723,9 +2708,21 @@
       <c r="T21">
         <v>420</v>
       </c>
-      <c r="AB21" s="2" t="e">
+      <c r="Y21">
+        <v>1500</v>
+      </c>
+      <c r="Z21">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="AA21">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="AB21" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-21.105381772844268</v>
+      </c>
+      <c r="AC21">
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
@@ -2776,9 +2773,21 @@
       <c r="T22">
         <v>430</v>
       </c>
-      <c r="AB22" s="2" t="e">
+      <c r="Y22">
+        <v>1600</v>
+      </c>
+      <c r="Z22">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AA22">
+        <v>3.9E-2</v>
+      </c>
+      <c r="AB22" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-21.712580051967343</v>
+      </c>
+      <c r="AC22">
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.25">
@@ -2829,9 +2838,21 @@
       <c r="T23">
         <v>470</v>
       </c>
-      <c r="AB23" s="2" t="e">
+      <c r="Y23">
+        <v>1700</v>
+      </c>
+      <c r="Z23">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="AA23">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="AB23" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-22.389516818135956</v>
+      </c>
+      <c r="AC23">
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
@@ -2882,9 +2903,21 @@
       <c r="T24">
         <v>500</v>
       </c>
-      <c r="AB24" s="2" t="e">
+      <c r="Y24">
+        <v>1750</v>
+      </c>
+      <c r="Z24">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="AA24">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AB24" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-22.615861927750718</v>
+      </c>
+      <c r="AC24">
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
@@ -2935,9 +2968,21 @@
       <c r="T25">
         <v>550</v>
       </c>
-      <c r="AB25" s="2" t="e">
+      <c r="Y25">
+        <v>1780</v>
+      </c>
+      <c r="Z25">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="AA25">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AB25" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-22.867644473911128</v>
+      </c>
+      <c r="AC25">
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.25">
@@ -2988,9 +3033,21 @@
       <c r="T26">
         <v>600</v>
       </c>
-      <c r="AB26" s="2" t="e">
+      <c r="Y26">
+        <v>1800</v>
+      </c>
+      <c r="Z26">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="AA26">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AB26" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-22.867644473911128</v>
+      </c>
+      <c r="AC26">
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
@@ -3041,9 +3098,21 @@
       <c r="T27">
         <v>650</v>
       </c>
-      <c r="AB27" s="2" t="e">
+      <c r="Y27">
+        <v>1900</v>
+      </c>
+      <c r="Z27">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="AA27">
+        <v>3.1E-2</v>
+      </c>
+      <c r="AB27" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-23.651606095996303</v>
+      </c>
+      <c r="AC27">
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.25">
@@ -3094,9 +3163,21 @@
       <c r="T28">
         <v>700</v>
       </c>
-      <c r="AB28" s="2" t="e">
+      <c r="Y28">
+        <v>2000</v>
+      </c>
+      <c r="Z28">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="AA28">
+        <v>0.03</v>
+      </c>
+      <c r="AB28" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-23.881031759908417</v>
+      </c>
+      <c r="AC28">
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.25">
@@ -3144,9 +3225,21 @@
         <f t="shared" si="8"/>
         <v>5.7781512503836439</v>
       </c>
-      <c r="AB29" s="2" t="e">
+      <c r="Y29">
+        <v>2500</v>
+      </c>
+      <c r="Z29">
+        <v>0.46</v>
+      </c>
+      <c r="AA29">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="AB29" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-26.810770738953096</v>
+      </c>
+      <c r="AC29">
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
@@ -3194,9 +3287,21 @@
         <f t="shared" si="8"/>
         <v>5.8129133566428557</v>
       </c>
-      <c r="AB30" s="2" t="e">
+      <c r="Y30">
+        <v>3000</v>
+      </c>
+      <c r="Z30">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="AA30">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AB30" s="2">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>-29.001131184440716</v>
+      </c>
+      <c r="AC30">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.25">
@@ -3457,10 +3562,6 @@
       <c r="H38">
         <f t="shared" si="3"/>
         <v>4.7923916894982534</v>
-      </c>
-      <c r="AB38" s="2" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>